<commit_message>
Completed placing order and signing out
</commit_message>
<xml_diff>
--- a/BeverageOrders/Orders.xlsx
+++ b/BeverageOrders/Orders.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908096D8-7038-4D35-BA1F-3C6D4D0B6272}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BEFD83-67A5-47B4-A1DE-9AD7486C17E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16900" windowHeight="7270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Product</t>
   </si>
@@ -83,7 +83,22 @@
     <t>Pot</t>
   </si>
   <si>
-    <t>700 W Mitchell Circle</t>
+    <t>700 W. Mitchell Cir</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Unable to find beveraged named 'Ipoh Coff'</t>
+  </si>
+  <si>
+    <t>Laughing Lumberjacks Lager</t>
+  </si>
+  <si>
+    <t>Unable to find beveraged named 'Laughing Lumberjacks Lager'</t>
   </si>
 </sst>
 </file>
@@ -119,9 +134,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,15 +423,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.36328125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -423,7 +445,7 @@
       <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -434,7 +456,10 @@
       <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -443,6 +468,9 @@
       <c r="B3" s="1">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -451,6 +479,9 @@
       <c r="B4" s="1">
         <v>4</v>
       </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -459,6 +490,9 @@
       <c r="B5" s="1">
         <v>1</v>
       </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -467,6 +501,9 @@
       <c r="B6" s="1">
         <v>2</v>
       </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
@@ -475,6 +512,9 @@
       <c r="B7" s="1">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -483,13 +523,47 @@
       <c r="B8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -502,7 +576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -547,7 +621,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="1">
-        <v>76014</v>
+        <v>76013</v>
       </c>
       <c r="E2" s="1">
         <v>253</v>

</xml_diff>

<commit_message>
Updated quantity set activity to check for available quantity before selecting.
</commit_message>
<xml_diff>
--- a/BeverageOrders/Orders.xlsx
+++ b/BeverageOrders/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BEFD83-67A5-47B4-A1DE-9AD7486C17E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2DF59D-3B71-47D5-AB71-B7CCA10FBA6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Product</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Unable to find beveraged named 'Laughing Lumberjacks Lager'</t>
+  </si>
+  <si>
+    <t>Quantity '2900' was unavailable</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -449,17 +452,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>2900</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
Added database and REST services. Also started on MVC front end.
</commit_message>
<xml_diff>
--- a/BeverageOrders/Orders.xlsx
+++ b/BeverageOrders/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2DF59D-3B71-47D5-AB71-B7CCA10FBA6E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC54F1F-607B-4DD4-B100-BA790C9D00F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,9 +35,6 @@
     <t>Ipoh Coffee</t>
   </si>
   <si>
-    <t>Sasquatch Ale</t>
-  </si>
-  <si>
     <t>Outback Lager</t>
   </si>
   <si>
@@ -101,7 +98,10 @@
     <t>Unable to find beveraged named 'Laughing Lumberjacks Lager'</t>
   </si>
   <si>
-    <t>Quantity '2900' was unavailable</t>
+    <t>Quantity '-50' was unavailable</t>
+  </si>
+  <si>
+    <t>Cote de Blaye</t>
   </si>
 </sst>
 </file>
@@ -428,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -446,10 +446,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -457,13 +457,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>2900</v>
+        <v>-50</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -474,101 +474,101 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1">
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -597,33 +597,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D2" s="1">
         <v>76013</v>

</xml_diff>

<commit_message>
Compeleted core project 2 automation logic
</commit_message>
<xml_diff>
--- a/BeverageOrders/Orders.xlsx
+++ b/BeverageOrders/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC54F1F-607B-4DD4-B100-BA790C9D00F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D766E549-D0CB-4869-A300-373AD49A0EB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Product</t>
   </si>
@@ -83,25 +83,10 @@
     <t>700 W. Mitchell Cir</t>
   </si>
   <si>
-    <t>Success</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>Unable to find beveraged named 'Ipoh Coff'</t>
-  </si>
-  <si>
-    <t>Laughing Lumberjacks Lager</t>
-  </si>
-  <si>
-    <t>Unable to find beveraged named 'Laughing Lumberjacks Lager'</t>
-  </si>
-  <si>
-    <t>Quantity '-50' was unavailable</t>
-  </si>
-  <si>
-    <t>Cote de Blaye</t>
+    <t>Rhonbrau Klosterbier</t>
+  </si>
+  <si>
+    <t>Not a real beverage lol</t>
   </si>
 </sst>
 </file>
@@ -426,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -452,19 +437,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>-50</v>
       </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -473,102 +453,77 @@
       <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
         <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="1">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
         <v>4</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated rest services quite a bit. Also got rpa product update working and order.xlsx mostly finished
</commit_message>
<xml_diff>
--- a/BeverageOrders/Orders.xlsx
+++ b/BeverageOrders/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D766E549-D0CB-4869-A300-373AD49A0EB4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F76B1B7-61D8-4BB9-8D24-0B675934B53A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Product</t>
   </si>
@@ -86,7 +86,7 @@
     <t>Rhonbrau Klosterbier</t>
   </si>
   <si>
-    <t>Not a real beverage lol</t>
+    <t>Not a real beverage</t>
   </si>
 </sst>
 </file>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,33 +496,17 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Full stack fully functional.
</commit_message>
<xml_diff>
--- a/BeverageOrders/Orders.xlsx
+++ b/BeverageOrders/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F76B1B7-61D8-4BB9-8D24-0B675934B53A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18972B6E-7272-4915-B63F-9491DEBC7D5D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Product</t>
   </si>
@@ -29,27 +29,24 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Chai</t>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Lakkalikoori</t>
+  </si>
+  <si>
+    <t>Chang</t>
   </si>
   <si>
     <t>Ipoh Coffee</t>
   </si>
   <si>
-    <t>Outback Lager</t>
-  </si>
-  <si>
-    <t>Guarana Fantastica</t>
-  </si>
-  <si>
-    <t>Steeleye Stout</t>
-  </si>
-  <si>
     <t>Laughing Lumberjack Lager</t>
   </si>
   <si>
-    <t>Ipoh Coff</t>
-  </si>
-  <si>
     <t>First Name</t>
   </si>
   <si>
@@ -68,12 +65,6 @@
     <t>Primary Phone</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -83,10 +74,13 @@
     <t>700 W. Mitchell Cir</t>
   </si>
   <si>
-    <t>Rhonbrau Klosterbier</t>
-  </si>
-  <si>
-    <t>Not a real beverage</t>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Unable to find beveraged named 'Ipoh Coffee'</t>
   </si>
 </sst>
 </file>
@@ -122,13 +116,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -414,13 +405,14 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A12" sqref="A12 A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.36328125" style="3" customWidth="1"/>
+    <col min="2" max="3" width="9.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.36328125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -431,85 +423,61 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>-50</v>
-      </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1">
-        <v>4</v>
-      </c>
-    </row>
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -521,7 +489,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F2" sqref="F2 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,33 +504,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1">
         <v>76013</v>

</xml_diff>

<commit_message>
Updated page layouts a bit.
</commit_message>
<xml_diff>
--- a/BeverageOrders/Orders.xlsx
+++ b/BeverageOrders/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18972B6E-7272-4915-B63F-9491DEBC7D5D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FDA999-7F0A-4AFF-A3DB-4AD061D628F6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,16 +35,16 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Lakkalikoori</t>
-  </si>
-  <si>
     <t>Chang</t>
   </si>
   <si>
-    <t>Ipoh Coffee</t>
-  </si>
-  <si>
-    <t>Laughing Lumberjack Lager</t>
+    <t>Cote de Blaye</t>
+  </si>
+  <si>
+    <t>Steeleye Stout</t>
+  </si>
+  <si>
+    <t>Rhonbrau Klosterbier</t>
   </si>
   <si>
     <t>First Name</t>
@@ -80,7 +80,7 @@
     <t>Failed</t>
   </si>
   <si>
-    <t>Unable to find beveraged named 'Ipoh Coffee'</t>
+    <t>Unable to find beveraged named 'Steeleye Stout'</t>
   </si>
 </sst>
 </file>
@@ -476,6 +476,7 @@
         <v>17</v>
       </c>
     </row>
+    <row r="6" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>

</xml_diff>